<commit_message>
Добавлен ktscrm/settings.py в .gitignore
</commit_message>
<xml_diff>
--- a/media/kuzets_download_ur.xlsx
+++ b/media/kuzets_download_ur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladislavkateryushin/Documents/crm-ktsNew-test/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF6A52-D1D4-E64A-9DC5-1DC3902C0842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51320EF6-63AA-0D40-A25A-BA17CAB3B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1486,7 +1486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2094,6 +2094,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -7721,7 +7724,7 @@
   <dimension ref="A1:S106"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:P7"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -8361,7 +8364,7 @@
     <row r="34" spans="1:16" s="120" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A34" s="41"/>
       <c r="B34" s="41"/>
-      <c r="C34" s="201"/>
+      <c r="C34" s="213"/>
       <c r="D34" s="202"/>
       <c r="E34" s="121"/>
       <c r="F34" s="118"/>

</xml_diff>